<commit_message>
Updated the FHIR Representation section to describe the mapping spreadsheet
</commit_message>
<xml_diff>
--- a/input/images/Mappings/M11 to FHIR Mapping 01.xlsx
+++ b/input/images/Mappings/M11 to FHIR Mapping 01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Filing\UDP\IG_HL7\input\images\Mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1162C3DF-4B3B-410B-AF63-8DE22345ED69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915F19A7-B8D4-4C3E-9F0A-48BA77B126E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{39AF0AD3-F111-4F4A-B4C7-6C1F6B3C7E56}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9004" uniqueCount="1661">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9004" uniqueCount="1662">
   <si>
     <t>M11</t>
   </si>
@@ -5726,6 +5726,9 @@
   </si>
   <si>
     <t>Purpose</t>
+  </si>
+  <si>
+    <t>Resource</t>
   </si>
 </sst>
 </file>
@@ -6684,7 +6687,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6784,7 +6787,7 @@
     </row>
     <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.45">
       <c r="A20" s="20" t="s">
-        <v>10</v>
+        <v>1661</v>
       </c>
       <c r="C20" t="s">
         <v>1640</v>
@@ -6828,8 +6831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27EFAB15-10D0-4095-9EA0-8CB6D97908A6}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A14" activeCellId="1" sqref="B15 A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7014,9 +7017,10 @@
     <hyperlink ref="B21" r:id="rId9" xr:uid="{3A37457B-AAD1-466C-99DD-B5326D84F5ED}"/>
     <hyperlink ref="B12" r:id="rId10" xr:uid="{8637737F-38BF-49FA-9748-B05C5F97EC4C}"/>
     <hyperlink ref="B10" r:id="rId11" xr:uid="{0E240F8F-EB77-40B2-9CDC-DDE1DE8DB0CC}"/>
+    <hyperlink ref="B15" r:id="rId12" xr:uid="{099D3171-EA74-44CB-989E-B10B61DC0C97}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -7024,8 +7028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68D01545-65CE-4DF7-B9C3-993F58E76E97}">
   <dimension ref="A1:Q676"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7112,7 +7116,7 @@
         <v>1277</v>
       </c>
       <c r="M4" s="20" t="s">
-        <v>10</v>
+        <v>1661</v>
       </c>
       <c r="N4" s="20" t="s">
         <v>12</v>
@@ -40358,17 +40362,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="433138c1-cfdf-4f6b-89e8-511447de8f15">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="50b1dd69-4c56-4a1c-b3ce-7cd2bac560be" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010062D9CD9ACC6AE244981CDEFACE8F40CE" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5588035a854d9997c1d7df24985cfe90">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="433138c1-cfdf-4f6b-89e8-511447de8f15" xmlns:ns3="50b1dd69-4c56-4a1c-b3ce-7cd2bac560be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="08b0b5a8a4dc2a6a7064cc49017e9875" ns2:_="" ns3:_="">
     <xsd:import namespace="433138c1-cfdf-4f6b-89e8-511447de8f15"/>
@@ -40597,6 +40590,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="433138c1-cfdf-4f6b-89e8-511447de8f15">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="50b1dd69-4c56-4a1c-b3ce-7cd2bac560be" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3C81A34-EC20-4306-AD93-063B9EE7A759}">
   <ds:schemaRefs>
@@ -40606,17 +40610,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B78000C0-76D0-4922-968B-4D7412227DA9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="433138c1-cfdf-4f6b-89e8-511447de8f15"/>
-    <ds:schemaRef ds:uri="50b1dd69-4c56-4a1c-b3ce-7cd2bac560be"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{88E36799-CA6B-4BDB-9F8A-B1B5CB126B31}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -40633,4 +40626,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B78000C0-76D0-4922-968B-4D7412227DA9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="433138c1-cfdf-4f6b-89e8-511447de8f15"/>
+    <ds:schemaRef ds:uri="50b1dd69-4c56-4a1c-b3ce-7cd2bac560be"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>